<commit_message>
Communication Module - SMS, WhatsApp, Email API changes
</commit_message>
<xml_diff>
--- a/Communication_API/SMSReport.xlsx
+++ b/Communication_API/SMSReport.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Admission Number</t>
   </si>
@@ -41,10 +41,10 @@
     <t>Grade 1-Section A</t>
   </si>
   <si>
-    <t>12/15/2024 00:00:00</t>
-  </si>
-  <si>
-    <t>Message is for Student 1</t>
+    <t>18 January 2025, 12:00 AM</t>
+  </si>
+  <si>
+    <t>Dear Aarav, your upcoming exam schedule is available. Please check the portal for details.</t>
   </si>
   <si>
     <t>Delivered</t>
@@ -56,10 +56,19 @@
     <t>Vivaan Raj Gupta</t>
   </si>
   <si>
-    <t>Message is for Student 2</t>
-  </si>
-  <si>
-    <t>Failed</t>
+    <t>Dear Vivaan, your upcoming exam schedule is available. Please check the portal for details.</t>
+  </si>
+  <si>
+    <t>Pending</t>
+  </si>
+  <si>
+    <t>ADM003</t>
+  </si>
+  <si>
+    <t>Aditya Singh Verma</t>
+  </si>
+  <si>
+    <t>Dear Aditya, your upcoming exam schedule is available. Please check the portal for details.</t>
   </si>
 </sst>
 </file>
@@ -106,7 +115,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr codeName=""/>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -172,6 +181,26 @@
         <v>15</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <headerFooter/>
 </worksheet>

</xml_diff>

<commit_message>
Communication Module - SMS, WhatApp, Email Export API
</commit_message>
<xml_diff>
--- a/Communication_API/SMSReport.xlsx
+++ b/Communication_API/SMSReport.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Admission Number</t>
   </si>
@@ -44,13 +44,16 @@
     <t>Grade 1-Section A</t>
   </si>
   <si>
-    <t>18 January 2025, 12:00 AM</t>
+    <t>04 February 2025, 12:00 AM</t>
   </si>
   <si>
-    <t>Dear Aarav, your upcoming exam schedule is available. Please check the portal for details.</t>
+    <t>Hi Student 1, This is a Test Message</t>
   </si>
   <si>
     <t>Delivered</t>
+  </si>
+  <si>
+    <t>John Smith</t>
   </si>
   <si>
     <t>ADM002</t>
@@ -59,28 +62,10 @@
     <t>Vivaan Raj Gupta</t>
   </si>
   <si>
-    <t>Dear Vivaan, your upcoming exam schedule is available. Please check the portal for details.</t>
+    <t>Hi Student 2, This is a Test Message</t>
   </si>
   <si>
     <t>Pending</t>
-  </si>
-  <si>
-    <t>ADM003</t>
-  </si>
-  <si>
-    <t>Aditya Singh Verma</t>
-  </si>
-  <si>
-    <t>Dear Aditya, your upcoming exam schedule is available. Please check the portal for details.</t>
-  </si>
-  <si>
-    <t>03 February 2025, 12:00 AM</t>
-  </si>
-  <si>
-    <t>Hi Student 1, This is a test message</t>
-  </si>
-  <si>
-    <t>John Smith</t>
   </si>
 </sst>
 </file>
@@ -127,7 +112,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr codeName=""/>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -175,14 +160,16 @@
       <c r="F2" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="G2"/>
+      <c r="G2" s="0" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>9</v>
@@ -191,55 +178,13 @@
         <v>10</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" s="0" t="s">
-        <v>22</v>
+      <c r="G3" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>